<commit_message>
Oct 12 - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>DATE</t>
   </si>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t>Ras-Pi session</t>
+  </si>
+  <si>
+    <t>12/10/2021</t>
+  </si>
+  <si>
+    <t>Compared the metadata of MP4,H264 and YUV</t>
+  </si>
+  <si>
+    <t>Share the notes</t>
+  </si>
+  <si>
+    <t>Self study on Android framework,Media Codec,BAYER filter ,Image processing</t>
+  </si>
+  <si>
+    <t>Fetching the hierarchy,layers and block diagrams</t>
+  </si>
+  <si>
+    <t>Revised all topics and ready to give session</t>
+  </si>
+  <si>
+    <t>Updated the notes</t>
+  </si>
+  <si>
+    <t>Internal discussion on V4L2 with the teammate</t>
   </si>
 </sst>
 </file>
@@ -75,9 +99,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -106,19 +130,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -130,13 +161,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,6 +189,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -205,6 +237,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -212,45 +251,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,19 +289,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,163 +469,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,15 +522,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -518,6 +533,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,150 +580,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1033,7 +1057,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1108,14 +1132,40 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="46.8" customHeight="1" spans="3:3">
-      <c r="C7" s="3"/>
+    <row r="7" ht="46.8" customHeight="1" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" ht="37.2" customHeight="1" spans="2:3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="10" ht="54.75" customHeight="1" spans="3:3">
+    <row r="9" spans="2:3">
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="54.75" customHeight="1" spans="2:3">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" ht="48" customHeight="1" spans="2:3">

</xml_diff>

<commit_message>
13 th  Oct - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>DATE</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>Internal discussion on V4L2 with the teammate</t>
+  </si>
+  <si>
+    <t>13/10/2021</t>
+  </si>
+  <si>
+    <t>Gave session on understanding so far</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  --  </t>
+  </si>
+  <si>
+    <t>Self study on frames,V4L2,NAL</t>
+  </si>
+  <si>
+    <t>Studying the test apps in detail</t>
+  </si>
+  <si>
+    <t>Tried all the 6 test apps and observed the output</t>
+  </si>
+  <si>
+    <t>Written own test app for open and uploaded to the GitHub</t>
   </si>
 </sst>
 </file>
@@ -99,10 +120,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -124,13 +145,51 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,36 +198,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,23 +225,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,9 +257,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,53 +279,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,181 +310,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,6 +501,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -500,24 +554,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,176 +601,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1054,10 +1075,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1168,14 +1189,38 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" ht="48" customHeight="1" spans="2:3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
+    <row r="11" ht="48" customHeight="1" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" ht="54.75" customHeight="1" spans="2:4">
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Oct 14 - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>DATE</t>
   </si>
@@ -112,7 +112,28 @@
     <t>Tried all the 6 test apps and observed the output</t>
   </si>
   <si>
+    <t>Exploring all testapps in detail</t>
+  </si>
+  <si>
     <t>Written own test app for open and uploaded to the GitHub</t>
+  </si>
+  <si>
+    <t>14/10/2021</t>
+  </si>
+  <si>
+    <t>Collected different logs using adb</t>
+  </si>
+  <si>
+    <t>Notes are updated</t>
+  </si>
+  <si>
+    <t>Internal discussion on Testapps with the teammate</t>
+  </si>
+  <si>
+    <t>Gave session on ARM programming in C</t>
+  </si>
+  <si>
+    <t>Obtained test app 1&amp; 2 by self after reffering the codes given</t>
   </si>
 </sst>
 </file>
@@ -120,10 +141,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -145,30 +166,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,39 +187,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,6 +217,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -233,17 +240,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,15 +262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,22 +279,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,187 +331,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,17 +525,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,15 +559,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,28 +578,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,149 +608,155 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1075,10 +1096,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1212,14 +1233,46 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:3">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="2:2">
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oct 18 - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>DATE</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t>Obtained test app 1&amp; 2 by self after reffering the codes given</t>
+  </si>
+  <si>
+    <t>15/10/2021</t>
+  </si>
+  <si>
+    <t>HOLIDAY</t>
+  </si>
+  <si>
+    <t>16/10/2021</t>
+  </si>
+  <si>
+    <t>17/10/2021</t>
+  </si>
+  <si>
+    <t>18/10/2021</t>
+  </si>
+  <si>
+    <t>Internal discussion with the teammate on testapps</t>
+  </si>
+  <si>
+    <t>Yet to push the testapps on to GitHub 1,2 pushed .</t>
+  </si>
+  <si>
+    <t>Completed till 4th testapp</t>
+  </si>
+  <si>
+    <t>Testapp 3  updated till format setting</t>
+  </si>
+  <si>
+    <t>Self study on V4L2 basics again,gone through the theory</t>
+  </si>
+  <si>
+    <t>Obtained different dumpsys logs using adb , need to push them to the repositry</t>
+  </si>
+  <si>
+    <t>V4L2 proprties,Structures and APIs are studied.</t>
+  </si>
+  <si>
+    <t>Attended ARM session on assembly code optimization</t>
   </si>
 </sst>
 </file>
@@ -141,8 +180,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -166,17 +205,30 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,8 +239,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,14 +249,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,32 +264,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,6 +308,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -285,6 +323,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -294,7 +340,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,14 +348,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,13 +370,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,43 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,37 +508,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,73 +544,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,35 +561,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -578,6 +588,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -589,6 +608,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,141 +650,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1096,13 +1135,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
@@ -1270,9 +1309,70 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" ht="108" customHeight="1" spans="2:2">
       <c r="B18" s="2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oct 19 - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>DATE</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>Attended ARM session on assembly code optimization</t>
+  </si>
+  <si>
+    <t>19/10/2021</t>
+  </si>
+  <si>
+    <t>Discussed with the teammate on testapps and v4l2</t>
+  </si>
+  <si>
+    <t>need to update logs collected by adb commands</t>
+  </si>
+  <si>
+    <t>All test apps are executed and uploaded to the GitHub</t>
+  </si>
+  <si>
+    <t>Revised the BT concepts</t>
+  </si>
+  <si>
+    <t>Self study on buffers,allocation,que-deque and device tree</t>
   </si>
 </sst>
 </file>
@@ -213,35 +231,72 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,20 +325,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -308,16 +349,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,37 +366,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,187 +388,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,8 +585,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,30 +656,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -653,149 +673,147 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1135,10 +1153,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1373,6 +1391,35 @@
     <row r="26" spans="2:2">
       <c r="B26" s="2" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20th Oct - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>DATE</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t>Self study on buffers,allocation,que-deque and device tree</t>
+  </si>
+  <si>
+    <t>20/10/2021</t>
+  </si>
+  <si>
+    <t>Updated all the testappswith kernel logs</t>
+  </si>
+  <si>
+    <t>Took guidance on Kernal logs</t>
   </si>
 </sst>
 </file>
@@ -198,8 +207,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -223,33 +232,35 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -257,54 +268,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,11 +321,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,31 +358,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,187 +397,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -579,15 +588,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -656,6 +656,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -685,135 +694,135 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1153,10 +1162,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1417,9 +1426,33 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:4">
       <c r="B30" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oct 21st - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
+    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>DATE</t>
   </si>
@@ -200,6 +200,27 @@
   </si>
   <si>
     <t>Took guidance on Kernal logs</t>
+  </si>
+  <si>
+    <t>21/10/2021</t>
+  </si>
+  <si>
+    <t>Studied all the kernel logs of V4L2 testapps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal discussion with the teammate </t>
+  </si>
+  <si>
+    <t>Going through V4L2 related links</t>
+  </si>
+  <si>
+    <t>Attended session on interrupt and ras-pi interrupt example</t>
+  </si>
+  <si>
+    <t>Listed all the doubts and posted the question</t>
+  </si>
+  <si>
+    <t>Completed the DS assignment given today and revising the BT topics.</t>
   </si>
 </sst>
 </file>
@@ -232,22 +253,142 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,127 +405,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -397,187 +418,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,32 +609,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -632,35 +627,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,146 +660,190 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -846,54 +867,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1162,19 +1183,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1453,6 +1474,43 @@
     <row r="33" spans="2:2">
       <c r="B33" s="2" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1474,9 +1532,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1494,9 +1552,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Oct 22nd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
+    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>DATE</t>
   </si>
@@ -221,6 +221,27 @@
   </si>
   <si>
     <t>Completed the DS assignment given today and revising the BT topics.</t>
+  </si>
+  <si>
+    <t>22/10/2021</t>
+  </si>
+  <si>
+    <t>Sync up meeting</t>
+  </si>
+  <si>
+    <t>Studying VBUF concepts</t>
+  </si>
+  <si>
+    <t>Doubts got cleared on buffers</t>
+  </si>
+  <si>
+    <t>Visualising the buffer concept and listing more doubts</t>
+  </si>
+  <si>
+    <t>Studied flows in the kernel space</t>
+  </si>
+  <si>
+    <t>Attended the session on Interrupts and Tasklets</t>
   </si>
 </sst>
 </file>
@@ -229,9 +250,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -253,11 +274,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -266,6 +287,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -273,6 +316,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -281,63 +332,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,8 +378,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -358,54 +417,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -418,19 +439,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,19 +565,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,139 +619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,6 +630,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -627,17 +672,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,190 +725,146 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -867,54 +888,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1183,19 +1204,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1378,7 +1399,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" ht="13" customHeight="1" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1447,7 +1468,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" ht="43" customHeight="1" spans="2:4">
       <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
@@ -1471,7 +1492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" ht="54" customHeight="1" spans="2:2">
       <c r="B33" s="2" t="s">
         <v>60</v>
       </c>
@@ -1508,9 +1529,41 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" ht="33" customHeight="1" spans="2:2">
       <c r="B38" s="2" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1532,9 +1585,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1552,9 +1605,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Oct 25th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
+    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>DATE</t>
   </si>
@@ -242,6 +242,36 @@
   </si>
   <si>
     <t>Attended the session on Interrupts and Tasklets</t>
+  </si>
+  <si>
+    <t>23/10/2021</t>
+  </si>
+  <si>
+    <t>24/10/2021</t>
+  </si>
+  <si>
+    <t>25/10/2021</t>
+  </si>
+  <si>
+    <t>yavta code lacking vcos header ,trying to fix it</t>
+  </si>
+  <si>
+    <t>Studied yavta code</t>
+  </si>
+  <si>
+    <t>Uploading the adb log files</t>
+  </si>
+  <si>
+    <t>Explored encode to file , on testapps</t>
+  </si>
+  <si>
+    <t>Explored more on ffmpeg</t>
+  </si>
+  <si>
+    <t>Attended Git session - internal discussion</t>
+  </si>
+  <si>
+    <t>Intenal discussion with the teammate</t>
   </si>
 </sst>
 </file>
@@ -249,10 +279,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -274,64 +304,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -340,10 +317,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -362,16 +370,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -385,6 +401,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,9 +416,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -408,16 +438,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -439,19 +469,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,37 +601,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,121 +649,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,6 +660,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -657,25 +711,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -698,173 +739,162 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -888,54 +918,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1204,19 +1234,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1564,6 +1594,61 @@
     <row r="42" spans="2:2">
       <c r="B42" s="2" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1585,9 +1670,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1605,9 +1690,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Oct 26th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t>DATE</t>
   </si>
@@ -272,6 +272,24 @@
   </si>
   <si>
     <t>Intenal discussion with the teammate</t>
+  </si>
+  <si>
+    <t>26/10/2021</t>
+  </si>
+  <si>
+    <t>Syncup on git link issue</t>
+  </si>
+  <si>
+    <t>editing the command on the yavta codes</t>
+  </si>
+  <si>
+    <t>clarified the doubts on the commads</t>
+  </si>
+  <si>
+    <t>Bugs in adb log files, trying to fix them</t>
+  </si>
+  <si>
+    <t>explored more on v4l2</t>
   </si>
 </sst>
 </file>
@@ -279,10 +297,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -304,11 +322,34 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -317,26 +358,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -348,113 +395,84 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,187 +487,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,6 +678,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -687,15 +720,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -707,17 +731,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -739,162 +752,167 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1234,10 +1252,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -1649,6 +1667,40 @@
     <row r="50" spans="2:2">
       <c r="B50" s="2" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oct 27th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
+    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
   <si>
     <t>DATE</t>
   </si>
@@ -290,6 +290,30 @@
   </si>
   <si>
     <t>explored more on v4l2</t>
+  </si>
+  <si>
+    <t>27/10/2021</t>
+  </si>
+  <si>
+    <t>Ran yavta code from the repositry but h264 not generated</t>
+  </si>
+  <si>
+    <t>Converting bin images to mp4 using ffmpeg</t>
+  </si>
+  <si>
+    <t>Explored more on ffmpeg commands</t>
+  </si>
+  <si>
+    <t>log files of yavta pushed to the GitHub ,need to clarify the doubts</t>
+  </si>
+  <si>
+    <t>Studied the cokor depth,chroma subsampling from basics</t>
+  </si>
+  <si>
+    <t>Explored the metadata and bitstream theory part</t>
+  </si>
+  <si>
+    <t>Studied BLE basics</t>
   </si>
 </sst>
 </file>
@@ -297,10 +321,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -322,6 +346,32 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -330,13 +380,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,21 +412,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,6 +448,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -397,15 +466,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,65 +501,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -487,13 +511,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,79 +637,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,19 +667,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,61 +691,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,6 +702,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -706,6 +745,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -720,32 +774,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -764,15 +797,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -781,138 +805,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -936,54 +960,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1252,19 +1276,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1701,6 +1725,40 @@
     <row r="55" spans="2:2">
       <c r="B55" s="2" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1722,9 +1780,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1742,9 +1800,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Oct 28th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
   <si>
     <t>DATE</t>
   </si>
@@ -314,6 +314,21 @@
   </si>
   <si>
     <t>Studied BLE basics</t>
+  </si>
+  <si>
+    <t>28/10/2021</t>
+  </si>
+  <si>
+    <t>We divided the yavta testapp as I analyzed the code and the teammate tried on the output debug</t>
+  </si>
+  <si>
+    <t>Studied each struct in yavta testapp listed 16 structs</t>
+  </si>
+  <si>
+    <t>Explored bytes perline</t>
+  </si>
+  <si>
+    <t>Exploring the v4l2 headers in yavta testapp</t>
   </si>
 </sst>
 </file>
@@ -321,10 +336,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -346,15 +361,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,15 +375,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,6 +392,13 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -412,7 +427,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -420,6 +467,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,41 +488,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -479,28 +516,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -517,19 +532,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,156 +707,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,16 +721,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -744,17 +759,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -777,8 +801,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -793,150 +817,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1276,10 +1291,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1759,6 +1774,30 @@
     <row r="60" spans="2:2">
       <c r="B60" s="2" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oct 29th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
+    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
   <si>
     <t>DATE</t>
   </si>
@@ -329,6 +329,24 @@
   </si>
   <si>
     <t>Exploring the v4l2 headers in yavta testapp</t>
+  </si>
+  <si>
+    <t>29/10/2021</t>
+  </si>
+  <si>
+    <t>Explored the yavta code</t>
+  </si>
+  <si>
+    <t>explored into the ffmpeg folder and tried executing</t>
+  </si>
+  <si>
+    <t>Listed the doubts to be cleared</t>
+  </si>
+  <si>
+    <t>./h264 executed and log files of i/p &amp; o/p are uploaded</t>
+  </si>
+  <si>
+    <t>Explored on hashing</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,15 +421,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -410,9 +445,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -433,14 +512,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -449,6 +520,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -456,66 +534,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -526,6 +544,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -538,25 +628,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,145 +682,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,21 +735,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -746,15 +749,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -784,6 +778,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -801,157 +821,155 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -975,54 +993,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1291,19 +1309,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1798,6 +1816,32 @@
       </c>
       <c r="C63" s="2" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1819,9 +1863,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1839,9 +1883,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Nov 1st - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
+    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="118">
   <si>
     <t>DATE</t>
   </si>
@@ -347,6 +347,30 @@
   </si>
   <si>
     <t>Explored on hashing</t>
+  </si>
+  <si>
+    <t>30/10/2021</t>
+  </si>
+  <si>
+    <t>31/10/2021</t>
+  </si>
+  <si>
+    <t>01/11/2021</t>
+  </si>
+  <si>
+    <t>Explored yavta app structures</t>
+  </si>
+  <si>
+    <t>Printed all possible struct members and metadata</t>
+  </si>
+  <si>
+    <t>Obtained the log and shared the GitHub link</t>
+  </si>
+  <si>
+    <t>discussion regarding the introduction to the module with the new teammate</t>
+  </si>
+  <si>
+    <t>Basics covered , self-revision</t>
   </si>
 </sst>
 </file>
@@ -355,9 +379,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -379,6 +403,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -387,13 +426,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -407,15 +477,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,17 +507,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,9 +538,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -468,72 +553,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -544,18 +568,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -568,25 +688,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,133 +742,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,6 +759,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -757,22 +820,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -803,30 +851,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -838,138 +862,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -993,54 +1017,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1309,19 +1333,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1842,6 +1866,53 @@
     <row r="67" spans="2:2">
       <c r="B67" s="2" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1863,9 +1934,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1883,9 +1954,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Nov 2nd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
+    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
   <si>
     <t>DATE</t>
   </si>
@@ -371,6 +371,21 @@
   </si>
   <si>
     <t>Basics covered , self-revision</t>
+  </si>
+  <si>
+    <t>02/11/2021</t>
+  </si>
+  <si>
+    <t>Internal discussion with the teammates</t>
+  </si>
+  <si>
+    <t>Uploaded the code exploring the structs in yavta , expected to complete all the structs by the end of tomorrow</t>
+  </si>
+  <si>
+    <t>Revision of C-DS-OS concepts</t>
+  </si>
+  <si>
+    <t>revised the basics from the docs and discussed all the topics with the new teammate</t>
   </si>
 </sst>
 </file>
@@ -378,10 +393,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -403,10 +418,62 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,9 +485,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,15 +516,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -454,21 +559,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -477,87 +567,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -568,187 +583,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,6 +774,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -777,11 +801,46 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -815,185 +874,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1017,54 +1032,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1333,19 +1348,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1913,6 +1928,25 @@
     <row r="74" spans="2:2">
       <c r="B74" s="2" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1934,9 +1968,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1954,9 +1988,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Nov 3rd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="127">
   <si>
     <t>DATE</t>
   </si>
@@ -386,6 +386,18 @@
   </si>
   <si>
     <t>revised the basics from the docs and discussed all the topics with the new teammate</t>
+  </si>
+  <si>
+    <t>Discussed in the group , got the doubts cleared on concepts finished till now</t>
+  </si>
+  <si>
+    <t>Started exploring the codec 2.0 and collected the useful links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Studying the collected pdfs on OPENMAX IL </t>
+  </si>
+  <si>
+    <t>Discussed doubts on ffmpeg with the new teammate</t>
   </si>
 </sst>
 </file>
@@ -393,9 +405,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -431,15 +443,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,6 +459,87 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -462,10 +549,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -477,14 +564,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -493,67 +572,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,13 +585,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -583,121 +595,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,61 +763,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,6 +798,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -801,30 +831,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -832,15 +838,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -856,6 +853,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,134 +889,134 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1012,7 +1024,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1027,6 +1039,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,10 +1363,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C62" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -1947,6 +1962,27 @@
     <row r="76" spans="2:2">
       <c r="B76" s="2" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="77" ht="31.5" spans="2:2">
+      <c r="B77" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 5th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="136">
   <si>
     <t>DATE</t>
   </si>
@@ -401,6 +401,30 @@
   </si>
   <si>
     <t>Discussed doubts on ffmpeg with the new teammate</t>
+  </si>
+  <si>
+    <t>04/11/2021</t>
+  </si>
+  <si>
+    <t>05/11/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continued on codec 2.0 </t>
+  </si>
+  <si>
+    <t>Revise the studied concepts and improve my understanding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listed the doubts , have to elaborate </t>
+  </si>
+  <si>
+    <t>Not a considerable progress but OPENMAX is reviewed and got understanding on the IL</t>
+  </si>
+  <si>
+    <t>Listed and observed the OPENMAX APIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Following android media architechture , observed abstractions in OPENMAX </t>
   </si>
 </sst>
 </file>
@@ -408,10 +432,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -431,6 +455,123 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -441,24 +582,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -469,17 +597,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -490,104 +612,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -598,187 +622,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,6 +813,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -804,8 +843,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -813,8 +867,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -834,32 +888,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -875,155 +903,151 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1366,10 +1390,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C67" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -1989,6 +2013,46 @@
     <row r="79" spans="2:2">
       <c r="B79" s="6" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 8th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
+    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="143">
   <si>
     <t>DATE</t>
   </si>
@@ -425,6 +425,27 @@
   </si>
   <si>
     <t xml:space="preserve">Following android media architechture , observed abstractions in OPENMAX </t>
+  </si>
+  <si>
+    <t>06/11/2021</t>
+  </si>
+  <si>
+    <t>07/11/2021</t>
+  </si>
+  <si>
+    <t>08/11/2021</t>
+  </si>
+  <si>
+    <t>Updating the notes</t>
+  </si>
+  <si>
+    <t>Reported the current study progress with refrerence and links</t>
+  </si>
+  <si>
+    <t>Attended the session on LDD recap</t>
+  </si>
+  <si>
+    <t>Had internal discussion with the teammates</t>
   </si>
 </sst>
 </file>
@@ -432,9 +453,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -458,7 +479,65 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,15 +559,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -501,10 +590,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -517,14 +620,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -537,81 +633,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -622,19 +643,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,19 +763,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,139 +799,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,6 +834,35 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -840,35 +890,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -889,165 +921,154 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1074,54 +1095,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1390,19 +1411,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C67" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -1991,7 +2012,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" ht="31.5" spans="1:2">
+    <row r="77" ht="30" spans="1:2">
       <c r="A77" s="1" t="s">
         <v>123</v>
       </c>
@@ -2053,6 +2074,48 @@
     <row r="84" spans="2:2">
       <c r="B84" s="2" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2074,9 +2137,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2094,9 +2157,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Nov 9th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="148">
   <si>
     <t>DATE</t>
   </si>
@@ -446,6 +446,21 @@
   </si>
   <si>
     <t>Had internal discussion with the teammates</t>
+  </si>
+  <si>
+    <t>09/11/2021</t>
+  </si>
+  <si>
+    <t>Explored on distinct layers of android multimedia framework</t>
+  </si>
+  <si>
+    <t>studied more on stagefright</t>
+  </si>
+  <si>
+    <t>Listed the links used for self study</t>
+  </si>
+  <si>
+    <t>Discussed and guided the new teammate on V4L2 testapps</t>
   </si>
 </sst>
 </file>
@@ -453,10 +468,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -480,6 +495,132 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,139 +634,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -633,6 +641,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -649,19 +664,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,157 +778,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,29 +854,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -905,17 +915,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -934,42 +938,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -978,97 +993,97 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1411,10 +1426,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2116,6 +2131,38 @@
     <row r="90" spans="2:2">
       <c r="B90" s="2" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 10th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="153">
   <si>
     <t>DATE</t>
   </si>
@@ -461,6 +461,21 @@
   </si>
   <si>
     <t>Discussed and guided the new teammate on V4L2 testapps</t>
+  </si>
+  <si>
+    <t>10/11/2021</t>
+  </si>
+  <si>
+    <t>Internal code-walkthrough on testapps</t>
+  </si>
+  <si>
+    <t>OpenMax : APIs ,Tunneling and components mechanism</t>
+  </si>
+  <si>
+    <t>Revising on BT,have to start C-DS-OS</t>
+  </si>
+  <si>
+    <t>Discussed doubts and progress in the group</t>
   </si>
 </sst>
 </file>
@@ -493,8 +508,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -514,27 +537,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,6 +550,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -579,13 +595,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -618,9 +627,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -634,14 +657,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -658,19 +673,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +805,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,37 +817,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,109 +853,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,26 +867,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,16 +940,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -952,138 +967,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1426,10 +1441,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2163,6 +2178,30 @@
     <row r="94" spans="2:2">
       <c r="B94" s="2" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="B96" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 11th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="158">
   <si>
     <t>DATE</t>
   </si>
@@ -476,6 +476,21 @@
   </si>
   <si>
     <t>Discussed doubts and progress in the group</t>
+  </si>
+  <si>
+    <t>11/11/2021</t>
+  </si>
+  <si>
+    <t>Attended the video basics ppt by thenew teammate</t>
+  </si>
+  <si>
+    <t>referring the shared links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discussed the doubts,installed yuv players </t>
+  </si>
+  <si>
+    <t>Attended the LDD recap session</t>
   </si>
 </sst>
 </file>
@@ -483,9 +498,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -506,6 +521,125 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -517,18 +651,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -536,114 +658,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,7 +673,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,13 +694,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,6 +790,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -709,37 +844,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,109 +856,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,25 +883,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -940,16 +946,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -967,138 +982,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1441,10 +1456,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2199,9 +2214,36 @@
         <v>151</v>
       </c>
     </row>
-    <row r="97" spans="2:2">
+    <row r="97" spans="2:4">
       <c r="B97" s="2" t="s">
         <v>152</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 12th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
+    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="164">
   <si>
     <t>DATE</t>
   </si>
@@ -491,6 +491,24 @@
   </si>
   <si>
     <t>Attended the LDD recap session</t>
+  </si>
+  <si>
+    <t>12/11/2021</t>
+  </si>
+  <si>
+    <t>Gone through the git repositries given and installed YUVview</t>
+  </si>
+  <si>
+    <t>Understood bitparsing with practical data and analysis through the application</t>
+  </si>
+  <si>
+    <t>Revision of previous topics</t>
+  </si>
+  <si>
+    <t>Tried FFMPEG as bit parser and uploaded the result file to the GitHub</t>
+  </si>
+  <si>
+    <t>OpenMax :Buffer,Enums,Callbacktype and functions</t>
   </si>
 </sst>
 </file>
@@ -498,10 +516,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -531,9 +549,104 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -546,20 +659,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -574,106 +691,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -688,13 +706,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,91 +874,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,73 +886,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,6 +897,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -893,6 +920,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -921,26 +963,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,152 +997,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1140,54 +1158,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1456,19 +1474,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C94" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -2057,7 +2075,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" ht="30" spans="1:2">
+    <row r="77" ht="31.5" spans="1:2">
       <c r="A77" s="1" t="s">
         <v>123</v>
       </c>
@@ -2244,6 +2262,35 @@
     <row r="100" spans="2:2">
       <c r="B100" s="2" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2265,9 +2312,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2285,9 +2332,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Nov 15th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
   <si>
     <t>DATE</t>
   </si>
@@ -509,6 +509,27 @@
   </si>
   <si>
     <t>OpenMax :Buffer,Enums,Callbacktype and functions</t>
+  </si>
+  <si>
+    <t>13/11/2021</t>
+  </si>
+  <si>
+    <t>14/11/2021</t>
+  </si>
+  <si>
+    <t>15/11/2021</t>
+  </si>
+  <si>
+    <t>OpenMax : Resource management,Buffer Payload</t>
+  </si>
+  <si>
+    <t>Internal discussion with teammates : Testapps</t>
+  </si>
+  <si>
+    <t>LDD recap session</t>
+  </si>
+  <si>
+    <t>16/11/2021</t>
   </si>
 </sst>
 </file>
@@ -516,10 +537,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -549,13 +570,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,24 +613,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -600,7 +629,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,15 +658,22 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -637,38 +688,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -682,18 +710,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -706,25 +727,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,157 +907,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,11 +921,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -924,6 +951,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -935,21 +971,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -974,6 +995,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -988,149 +1018,140 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1474,10 +1495,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C94" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -2291,6 +2312,51 @@
     <row r="104" spans="2:2">
       <c r="B104" s="2" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov - 16th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19500" windowHeight="7890" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="175">
   <si>
     <t>DATE</t>
   </si>
@@ -530,6 +530,18 @@
   </si>
   <si>
     <t>16/11/2021</t>
+  </si>
+  <si>
+    <t>OpenMax : Revision,Image Video common</t>
+  </si>
+  <si>
+    <t>Low level android media APIs</t>
+  </si>
+  <si>
+    <t>Media Player,Codecs</t>
+  </si>
+  <si>
+    <t>Internal  discussion with teammates on yavta and run.sh file copmmands</t>
   </si>
 </sst>
 </file>
@@ -537,10 +549,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -562,40 +574,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
@@ -607,96 +595,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -717,6 +616,119 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -727,13 +739,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,37 +847,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,90 +901,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -878,36 +920,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,6 +930,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -932,6 +992,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -954,205 +1025,146 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1179,54 +1191,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1495,19 +1507,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.44" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.4380952380952" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.6666666666667" style="2" customWidth="1"/>
     <col min="3" max="3" width="54" style="2" customWidth="1"/>
     <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="5" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.6" customHeight="1" spans="1:4">
@@ -2096,7 +2108,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" ht="31.5" spans="1:2">
+    <row r="77" ht="30" spans="1:2">
       <c r="A77" s="1" t="s">
         <v>123</v>
       </c>
@@ -2354,9 +2366,33 @@
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
         <v>170</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2378,9 +2414,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2398,9 +2434,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.52666666666667" customWidth="1"/>
+    <col min="1" max="1025" width="8.52380952380952" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Nov 17th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="180">
   <si>
     <t>DATE</t>
   </si>
@@ -542,6 +542,21 @@
   </si>
   <si>
     <t>Internal  discussion with teammates on yavta and run.sh file copmmands</t>
+  </si>
+  <si>
+    <t>17/11/2021</t>
+  </si>
+  <si>
+    <t>Reported the progress of openmax and codec 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal discussion with the teammates on ppt </t>
+  </si>
+  <si>
+    <t>Preparing the codec 2.0 ppt</t>
+  </si>
+  <si>
+    <t>Revised basic C concepts with the teammate</t>
   </si>
 </sst>
 </file>
@@ -549,10 +564,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -574,21 +589,28 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -596,45 +618,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -649,7 +632,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -663,23 +646,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -694,7 +701,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -702,14 +709,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -729,6 +729,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -739,31 +754,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,151 +922,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,6 +945,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -944,6 +998,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,32 +1029,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1006,165 +1045,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1507,10 +1522,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2393,6 +2408,27 @@
     <row r="113" spans="2:2">
       <c r="B113" s="2" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="B115" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 18th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="185">
   <si>
     <t>DATE</t>
   </si>
@@ -557,6 +557,21 @@
   </si>
   <si>
     <t>Revised basic C concepts with the teammate</t>
+  </si>
+  <si>
+    <t>18/11/2021</t>
+  </si>
+  <si>
+    <t>Prepared the ppt on OpenMax</t>
+  </si>
+  <si>
+    <t>Internally discussed with the teammates on Android media framework</t>
+  </si>
+  <si>
+    <t>Prepared unified ppt of the team</t>
+  </si>
+  <si>
+    <t>Revised the Android multimedia concepts</t>
   </si>
 </sst>
 </file>
@@ -564,10 +579,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -589,24 +604,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -623,6 +631,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -632,7 +656,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -640,15 +664,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -700,24 +716,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -732,14 +747,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,25 +769,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,157 +937,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -945,6 +960,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1011,6 +1037,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1025,62 +1060,42 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1089,97 +1104,97 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1522,10 +1537,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2429,6 +2444,32 @@
     <row r="116" spans="2:2">
       <c r="B116" s="2" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 19th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="190">
   <si>
     <t>DATE</t>
   </si>
@@ -572,6 +572,21 @@
   </si>
   <si>
     <t>Revised the Android multimedia concepts</t>
+  </si>
+  <si>
+    <t>19/11/2021</t>
+  </si>
+  <si>
+    <t>Prepared to give ppt on OpenMax on Monday</t>
+  </si>
+  <si>
+    <t>Internally discussed on Interview questions</t>
+  </si>
+  <si>
+    <t>Prepared to give Memory management session on next week</t>
+  </si>
+  <si>
+    <t>Revised on Stagefright and OpenMax</t>
   </si>
 </sst>
 </file>
@@ -579,10 +594,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -604,21 +619,21 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -639,16 +654,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -657,6 +673,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -700,14 +723,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -716,16 +731,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -739,7 +746,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,7 +761,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -769,25 +784,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,157 +952,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -960,6 +975,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -974,17 +998,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1028,20 +1046,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1066,135 +1081,135 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1537,10 +1552,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2470,6 +2485,27 @@
     <row r="120" spans="2:2">
       <c r="B120" s="2" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3">
+      <c r="B122" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 22nd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="197">
   <si>
     <t>DATE</t>
   </si>
@@ -587,6 +587,27 @@
   </si>
   <si>
     <t>Revised on Stagefright and OpenMax</t>
+  </si>
+  <si>
+    <t>20/11/2021</t>
+  </si>
+  <si>
+    <t>21/11/2021</t>
+  </si>
+  <si>
+    <t>22/11/2021</t>
+  </si>
+  <si>
+    <t>Internal discussion on Memory management concepts</t>
+  </si>
+  <si>
+    <t>Preparing ppt on Memory Management</t>
+  </si>
+  <si>
+    <t>Prepared to give session on OpenMax</t>
+  </si>
+  <si>
+    <t>Revising on basic C-DS-OS concepts</t>
   </si>
 </sst>
 </file>
@@ -594,9 +615,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -619,19 +640,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -639,14 +647,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -662,24 +662,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -701,17 +706,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -723,18 +729,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -754,7 +761,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -767,13 +774,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -784,49 +805,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,132 +986,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,27 +1003,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1022,15 +1038,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1042,6 +1049,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1061,155 +1077,160 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1552,10 +1573,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2506,6 +2527,41 @@
     <row r="123" spans="2:2">
       <c r="B123" s="2" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3">
+      <c r="B127" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 23rd -  Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="202">
   <si>
     <t>DATE</t>
   </si>
@@ -608,6 +608,21 @@
   </si>
   <si>
     <t>Revising on basic C-DS-OS concepts</t>
+  </si>
+  <si>
+    <t>23/11/2021</t>
+  </si>
+  <si>
+    <t>Gave ppt on OpenMax</t>
+  </si>
+  <si>
+    <t>Preparing on the Multi level Paging and Inverted Paging</t>
+  </si>
+  <si>
+    <t>Gave session on Memory management for freshers and interns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Going through the android xref links sent </t>
   </si>
 </sst>
 </file>
@@ -617,8 +632,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -647,11 +662,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -662,11 +690,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -675,16 +698,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,18 +730,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -729,9 +752,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -745,8 +767,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -759,9 +782,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -775,21 +805,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -805,187 +820,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1009,16 +1024,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1056,23 +1071,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1080,8 +1080,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1096,141 +1096,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1573,10 +1588,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2562,6 +2577,28 @@
       </c>
       <c r="C127" s="2" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3">
+      <c r="B129" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 24th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="204">
   <si>
     <t>DATE</t>
   </si>
@@ -623,6 +623,12 @@
   </si>
   <si>
     <t xml:space="preserve">Going through the android xref links sent </t>
+  </si>
+  <si>
+    <t>24/11/2021</t>
+  </si>
+  <si>
+    <t>Gave session to the freshers on MM-2 along with the teammate</t>
   </si>
 </sst>
 </file>
@@ -630,10 +636,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -655,16 +661,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -677,9 +704,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -701,22 +738,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -752,24 +773,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -783,7 +796,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -791,21 +811,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,187 +826,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,7 +1024,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1054,6 +1060,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1079,15 +1109,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1096,156 +1117,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1588,10 +1594,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2599,6 +2605,22 @@
       </c>
       <c r="C129" s="2" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3">
+      <c r="C131" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 25th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="209">
   <si>
     <t>DATE</t>
   </si>
@@ -629,6 +629,21 @@
   </si>
   <si>
     <t>Gave session to the freshers on MM-2 along with the teammate</t>
+  </si>
+  <si>
+    <t>25/11/2021</t>
+  </si>
+  <si>
+    <t>Configured the VPN</t>
+  </si>
+  <si>
+    <t>Attended the ADB session with freshers</t>
+  </si>
+  <si>
+    <t>Revising the basic OS concepts</t>
+  </si>
+  <si>
+    <t>Media Player/Services android codes and android xref</t>
   </si>
 </sst>
 </file>
@@ -636,9 +651,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -661,14 +676,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -678,15 +685,10 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -705,15 +707,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -727,11 +740,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -773,18 +786,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -795,8 +801,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -832,25 +847,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -862,19 +985,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,127 +1021,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,21 +1040,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1060,16 +1060,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,6 +1098,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1120,72 +1135,72 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1194,64 +1209,64 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1594,10 +1609,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2618,9 +2633,28 @@
         <v>201</v>
       </c>
     </row>
-    <row r="131" spans="3:3">
+    <row r="131" spans="1:3">
+      <c r="A131" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="C131" s="2" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3">
+      <c r="B132" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3">
+      <c r="C133" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 26th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="214">
   <si>
     <t>DATE</t>
   </si>
@@ -644,6 +644,21 @@
   </si>
   <si>
     <t>Media Player/Services android codes and android xref</t>
+  </si>
+  <si>
+    <t>26/11/2021</t>
+  </si>
+  <si>
+    <t>Gone through android codes shared</t>
+  </si>
+  <si>
+    <t>Interview preparation</t>
+  </si>
+  <si>
+    <t>Attempted the interview questions and uploaded to the git</t>
+  </si>
+  <si>
+    <t>OS and LDD revision</t>
   </si>
 </sst>
 </file>
@@ -651,9 +666,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -676,8 +691,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,23 +707,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,37 +726,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -778,6 +764,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -786,11 +779,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -818,7 +826,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -831,6 +839,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -841,25 +856,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,157 +1000,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,21 +1074,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1099,6 +1099,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1109,15 +1133,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1135,48 +1150,48 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1185,88 +1200,88 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1609,10 +1624,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2655,6 +2670,25 @@
     <row r="133" spans="3:3">
       <c r="C133" s="2" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3">
+      <c r="B135" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 29th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="220">
   <si>
     <t>DATE</t>
   </si>
@@ -659,6 +659,24 @@
   </si>
   <si>
     <t>OS and LDD revision</t>
+  </si>
+  <si>
+    <t>27/11/2021</t>
+  </si>
+  <si>
+    <t>28/11/2021</t>
+  </si>
+  <si>
+    <t>29/11/2021</t>
+  </si>
+  <si>
+    <t>Revising basic CPP and OOPs concepts</t>
+  </si>
+  <si>
+    <t>Tried Logical and Puzzle questions</t>
+  </si>
+  <si>
+    <t>Preparing for the interview</t>
   </si>
 </sst>
 </file>
@@ -667,9 +685,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -691,9 +709,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -707,13 +730,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,9 +760,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,6 +778,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -751,6 +806,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -758,7 +828,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -779,44 +849,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -825,23 +857,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -856,187 +874,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,11 +1068,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,6 +1142,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1112,176 +1165,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1624,10 +1642,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2689,6 +2707,41 @@
       </c>
       <c r="C135" s="2" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3">
+      <c r="B139" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov 30th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="226">
   <si>
     <t>DATE</t>
   </si>
@@ -677,6 +677,24 @@
   </si>
   <si>
     <t>Preparing for the interview</t>
+  </si>
+  <si>
+    <t>30/11/2021</t>
+  </si>
+  <si>
+    <t>Attended the bench meet</t>
+  </si>
+  <si>
+    <t>MediaPlayer, Media codec and MPEG4 writer codes ,an overview and studied the variables</t>
+  </si>
+  <si>
+    <t>Tried interview questions</t>
+  </si>
+  <si>
+    <t>OS concepts and LDD revision</t>
+  </si>
+  <si>
+    <t>01/12/2021</t>
   </si>
 </sst>
 </file>
@@ -684,10 +702,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -709,33 +727,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -760,16 +761,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -778,20 +772,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -806,7 +786,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,10 +823,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -841,11 +853,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -856,14 +882,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -874,37 +892,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,13 +1018,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -934,127 +1042,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,41 +1083,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1145,6 +1128,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1165,141 +1168,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1642,10 +1660,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2742,6 +2760,37 @@
       </c>
       <c r="C139" s="2" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3">
+      <c r="B142" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3">
+      <c r="C143" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 1st - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="8580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="229">
   <si>
     <t>DATE</t>
   </si>
@@ -695,6 +695,15 @@
   </si>
   <si>
     <t>01/12/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal discussion on the codes shared </t>
+  </si>
+  <si>
+    <t>Tried the question shared in the group from the interview</t>
+  </si>
+  <si>
+    <t>Solving logical puzzles</t>
   </si>
 </sst>
 </file>
@@ -702,10 +711,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -728,7 +737,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,18 +763,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -780,13 +789,6 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -831,6 +833,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,43 +891,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -892,103 +901,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,79 +1069,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,6 +1092,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1110,46 +1134,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1183,141 +1172,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1660,10 +1669,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2788,9 +2797,28 @@
         <v>219</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
         <v>225</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3">
+      <c r="B145" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3">
+      <c r="C146" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 2nd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8580" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="233">
   <si>
     <t>DATE</t>
   </si>
@@ -704,6 +704,18 @@
   </si>
   <si>
     <t>Solving logical puzzles</t>
+  </si>
+  <si>
+    <t>02/12/2021</t>
+  </si>
+  <si>
+    <t>Internal discussion on puzzles questions</t>
+  </si>
+  <si>
+    <t>Continuing with the android media codes</t>
+  </si>
+  <si>
+    <t>03/12/2021</t>
   </si>
 </sst>
 </file>
@@ -711,9 +723,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -736,8 +748,36 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -751,28 +791,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -795,17 +830,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -818,30 +867,16 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -856,30 +891,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -901,25 +913,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,157 +1075,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,16 +1108,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1134,6 +1146,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1143,17 +1170,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1175,17 +1198,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1195,138 +1207,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1669,10 +1681,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2819,6 +2831,27 @@
     <row r="146" spans="3:3">
       <c r="C146" s="2" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3">
+      <c r="C148" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 3rd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="241">
   <si>
     <t>DATE</t>
   </si>
@@ -716,6 +716,30 @@
   </si>
   <si>
     <t>03/12/2021</t>
+  </si>
+  <si>
+    <t>Revised basic C programming</t>
+  </si>
+  <si>
+    <t>LDD-DS-OS concepts</t>
+  </si>
+  <si>
+    <t>Interview questions</t>
+  </si>
+  <si>
+    <t>04/12/2021</t>
+  </si>
+  <si>
+    <t>05/12/2021</t>
+  </si>
+  <si>
+    <t>06/12/2021</t>
+  </si>
+  <si>
+    <t>LEAVE</t>
+  </si>
+  <si>
+    <t>07/12/2021</t>
   </si>
 </sst>
 </file>
@@ -723,9 +747,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -748,19 +772,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -770,14 +785,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,7 +807,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -806,8 +821,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -845,16 +861,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -868,7 +885,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -883,15 +908,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -903,6 +920,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -913,13 +937,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,169 +1099,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,6 +1142,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1170,17 +1205,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1207,138 +1231,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1681,10 +1705,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E149"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2849,9 +2873,52 @@
         <v>231</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
         <v>232</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3">
+      <c r="B150" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 7th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="244">
   <si>
     <t>DATE</t>
   </si>
@@ -740,6 +740,15 @@
   </si>
   <si>
     <t>07/12/2021</t>
+  </si>
+  <si>
+    <t>Basic C revision</t>
+  </si>
+  <si>
+    <t>Revising OS and preparing for the interview</t>
+  </si>
+  <si>
+    <t>08/12/2021</t>
   </si>
 </sst>
 </file>
@@ -747,10 +756,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -773,15 +782,115 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -798,24 +907,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -829,104 +930,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -937,13 +946,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -955,169 +1114,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1128,6 +1137,69 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1157,69 +1229,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1231,138 +1240,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1705,10 +1714,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2916,9 +2925,20 @@
         <v>239</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
         <v>240</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 8th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="246">
   <si>
     <t>DATE</t>
   </si>
@@ -749,6 +749,12 @@
   </si>
   <si>
     <t>08/12/2021</t>
+  </si>
+  <si>
+    <t>Preparing on OS concepts for discussion tommorow morning</t>
+  </si>
+  <si>
+    <t>09/12/2021</t>
   </si>
 </sst>
 </file>
@@ -756,10 +762,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -781,8 +787,59 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -790,6 +847,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -804,59 +883,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -871,37 +914,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -916,22 +930,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -946,7 +952,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -958,7 +970,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -970,7 +988,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,7 +1000,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,31 +1066,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,85 +1120,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1121,12 +1133,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,31 +1150,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1189,16 +1171,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1214,6 +1205,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1240,138 +1246,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1714,10 +1720,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2936,9 +2942,23 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:3">
       <c r="A155" s="1" t="s">
         <v>243</v>
+      </c>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3">
+      <c r="C156" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decd 9th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="249">
   <si>
     <t>DATE</t>
   </si>
@@ -755,6 +755,15 @@
   </si>
   <si>
     <t>09/12/2021</t>
+  </si>
+  <si>
+    <t>Interview question discussion</t>
+  </si>
+  <si>
+    <t>Preparing for the discussion on interview question tomorrow.</t>
+  </si>
+  <si>
+    <t>10/12/2021</t>
   </si>
 </sst>
 </file>
@@ -762,10 +771,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -787,9 +796,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -799,8 +836,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -816,7 +854,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -830,14 +883,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -847,31 +892,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -884,7 +915,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -898,13 +929,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -913,9 +937,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -928,20 +951,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -949,6 +958,150 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -958,13 +1111,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,163 +1141,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,30 +1152,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1188,8 +1173,52 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1223,161 +1252,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1720,10 +1729,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2946,7 +2955,6 @@
       <c r="A155" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B155" s="2"/>
       <c r="C155" s="2" t="s">
         <v>211</v>
       </c>
@@ -2956,9 +2964,25 @@
         <v>244</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
         <v>245</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3">
+      <c r="C158" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 10th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="253">
   <si>
     <t>DATE</t>
   </si>
@@ -764,6 +764,18 @@
   </si>
   <si>
     <t>10/12/2021</t>
+  </si>
+  <si>
+    <t>Going through my resume</t>
+  </si>
+  <si>
+    <t>11/12/2021</t>
+  </si>
+  <si>
+    <t>12/12/2021</t>
+  </si>
+  <si>
+    <t>13/12/2021</t>
   </si>
 </sst>
 </file>
@@ -771,10 +783,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -797,7 +809,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -809,21 +821,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -836,17 +834,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -860,6 +873,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -884,23 +898,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,24 +928,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -944,9 +949,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -961,19 +973,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,19 +1075,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1009,25 +1129,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,109 +1147,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1152,6 +1164,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1170,11 +1206,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1206,8 +1248,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1222,171 +1264,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1729,10 +1741,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2980,9 +2992,38 @@
         <v>247</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:3">
       <c r="A159" s="1" t="s">
         <v>248</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3">
+      <c r="C160" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 13th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="255">
   <si>
     <t>DATE</t>
   </si>
@@ -776,6 +776,12 @@
   </si>
   <si>
     <t>13/12/2021</t>
+  </si>
+  <si>
+    <t>Discussion of interview questions with Team-3</t>
+  </si>
+  <si>
+    <t>Attended session on OS introduction,Process management and Process states</t>
   </si>
 </sst>
 </file>
@@ -784,9 +790,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -808,10 +814,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -821,7 +828,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -834,29 +841,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -865,9 +849,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,15 +896,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -928,8 +918,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -943,6 +950,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -950,15 +964,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -973,7 +979,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,37 +1081,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,133 +1159,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1164,45 +1170,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1245,11 +1212,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1264,141 +1237,174 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1741,10 +1747,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3021,9 +3027,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
         <v>252</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 14th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="258">
   <si>
     <t>DATE</t>
   </si>
@@ -782,6 +782,15 @@
   </si>
   <si>
     <t>Attended session on OS introduction,Process management and Process states</t>
+  </si>
+  <si>
+    <t>14/12/2021</t>
+  </si>
+  <si>
+    <t>Output of the C-Programs,OS concepts and LDD</t>
+  </si>
+  <si>
+    <t>15/12/2021</t>
   </si>
 </sst>
 </file>
@@ -789,9 +798,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -814,6 +823,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -822,20 +843,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -850,9 +867,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -866,14 +883,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -896,9 +905,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -920,23 +929,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -949,8 +956,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -962,13 +978,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -976,6 +985,96 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -985,31 +1084,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,25 +1132,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,31 +1150,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1087,79 +1162,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,6 +1193,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1212,28 +1236,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1241,8 +1248,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1264,147 +1271,149 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1747,10 +1756,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3041,6 +3050,24 @@
     <row r="164" spans="2:2">
       <c r="B164" s="2" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 15th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="261">
   <si>
     <t>DATE</t>
   </si>
@@ -791,6 +791,15 @@
   </si>
   <si>
     <t>15/12/2021</t>
+  </si>
+  <si>
+    <t>Attended the interview</t>
+  </si>
+  <si>
+    <t>Shared the questions to the teammates for the reference</t>
+  </si>
+  <si>
+    <t>16/12/2021</t>
   </si>
 </sst>
 </file>
@@ -799,9 +808,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -823,24 +832,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -850,9 +844,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -866,31 +859,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -905,9 +884,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -916,6 +895,21 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -936,20 +930,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -959,6 +939,35 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,7 +997,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,19 +1075,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,7 +1093,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,139 +1177,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,36 +1188,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1236,6 +1215,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1245,11 +1239,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1271,6 +1271,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1282,138 +1291,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1756,10 +1765,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3065,9 +3074,22 @@
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:2">
       <c r="A167" s="1" t="s">
         <v>257</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 16th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="264">
   <si>
     <t>DATE</t>
   </si>
@@ -800,6 +800,15 @@
   </si>
   <si>
     <t>16/12/2021</t>
+  </si>
+  <si>
+    <t>Questions shared by the teammates</t>
+  </si>
+  <si>
+    <t>Programming practice</t>
+  </si>
+  <si>
+    <t>17/12/2021</t>
   </si>
 </sst>
 </file>
@@ -809,8 +818,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -844,37 +853,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -884,9 +862,40 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -906,10 +915,33 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -921,16 +953,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -951,28 +989,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,13 +996,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -994,6 +1003,66 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1003,13 +1072,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,43 +1174,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,114 +1187,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1188,6 +1197,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1209,23 +1257,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1235,21 +1268,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1271,15 +1289,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1291,138 +1300,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1765,10 +1774,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3087,9 +3096,22 @@
         <v>259</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
         <v>260</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3">
+      <c r="C170" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 17th - Statsus
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="266">
   <si>
     <t>DATE</t>
   </si>
@@ -809,6 +809,12 @@
   </si>
   <si>
     <t>17/12/2021</t>
+  </si>
+  <si>
+    <t>Revising the DS concepts</t>
+  </si>
+  <si>
+    <t>18/12/2021</t>
   </si>
 </sst>
 </file>
@@ -816,9 +822,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -841,13 +847,79 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,8 +933,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -877,120 +997,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1006,7 +1012,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,7 +1036,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,13 +1060,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,13 +1084,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,7 +1120,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,115 +1186,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1197,30 +1203,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1235,6 +1217,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1257,17 +1248,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1287,6 +1269,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1300,138 +1306,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1774,10 +1780,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E171"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+      <selection activeCell="A173" sqref="A173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3109,9 +3115,22 @@
         <v>262</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
         <v>263</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3">
+      <c r="C172" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 20th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="272">
   <si>
     <t>DATE</t>
   </si>
@@ -815,6 +815,24 @@
   </si>
   <si>
     <t>18/12/2021</t>
+  </si>
+  <si>
+    <t>19/12/2021</t>
+  </si>
+  <si>
+    <t>20/12/2021</t>
+  </si>
+  <si>
+    <t>Solving all the programming questions asked in interviews</t>
+  </si>
+  <si>
+    <t>Trying different approach</t>
+  </si>
+  <si>
+    <t>Solving the puzzle questions too</t>
+  </si>
+  <si>
+    <t>21/12/2021</t>
   </si>
 </sst>
 </file>
@@ -822,9 +840,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -847,18 +865,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -875,7 +894,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -883,13 +902,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -903,33 +915,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -941,25 +945,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -982,7 +970,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1002,6 +990,36 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1012,7 +1030,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,13 +1144,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,61 +1162,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,85 +1198,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1203,30 +1221,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1255,16 +1249,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1286,15 +1298,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1303,141 +1306,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1780,10 +1798,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3128,9 +3146,43 @@
         <v>264</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:2">
       <c r="A173" s="1" t="s">
         <v>265</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3">
+      <c r="C176" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3">
+      <c r="C177" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 21st - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="275">
   <si>
     <t>DATE</t>
   </si>
@@ -833,6 +833,15 @@
   </si>
   <si>
     <t>21/12/2021</t>
+  </si>
+  <si>
+    <t>Continued solving the programming questions</t>
+  </si>
+  <si>
+    <t>Revising DS and trying Que programs</t>
+  </si>
+  <si>
+    <t>22/12/2021</t>
   </si>
 </sst>
 </file>
@@ -840,9 +849,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -865,9 +874,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -881,9 +894,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -894,22 +933,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,13 +969,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -945,9 +977,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -970,22 +1001,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1013,13 +1029,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1030,7 +1039,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,37 +1063,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1090,31 +1105,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,7 +1141,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,25 +1177,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1174,25 +1195,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,7 +1219,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1221,6 +1230,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1263,24 +1292,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1298,11 +1309,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1324,138 +1333,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1798,10 +1807,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3180,9 +3189,22 @@
         <v>270</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
         <v>271</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3">
+      <c r="C179" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 22nd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="286">
   <si>
     <t>DATE</t>
   </si>
@@ -842,6 +842,39 @@
   </si>
   <si>
     <t>22/12/2021</t>
+  </si>
+  <si>
+    <t>Revised the OS:Process,IPC</t>
+  </si>
+  <si>
+    <t>DS:Que programs</t>
+  </si>
+  <si>
+    <t>23/12/2021</t>
+  </si>
+  <si>
+    <t>24/12/2021</t>
+  </si>
+  <si>
+    <t>25/12/2021</t>
+  </si>
+  <si>
+    <t>26/12/2021</t>
+  </si>
+  <si>
+    <t>27/12/2021</t>
+  </si>
+  <si>
+    <t>28/12/2021</t>
+  </si>
+  <si>
+    <t>29/12/2021</t>
+  </si>
+  <si>
+    <t>30/12/2021</t>
+  </si>
+  <si>
+    <t>31/12/2021</t>
   </si>
 </sst>
 </file>
@@ -849,9 +882,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -874,13 +907,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -896,22 +924,26 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -925,30 +957,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -970,6 +981,28 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -977,38 +1010,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1029,6 +1040,28 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1039,7 +1072,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,7 +1096,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,18 +1132,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1093,7 +1144,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1105,43 +1228,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,73 +1246,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1235,20 +1268,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1292,6 +1314,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1303,15 +1334,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1330,141 +1352,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1807,10 +1840,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+      <selection activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3202,9 +3235,62 @@
         <v>273</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
         <v>274</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3">
+      <c r="C181" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 23rd - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="8580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="280">
   <si>
     <t>DATE</t>
   </si>
@@ -853,28 +853,10 @@
     <t>23/12/2021</t>
   </si>
   <si>
-    <t>24/12/2021</t>
-  </si>
-  <si>
-    <t>25/12/2021</t>
-  </si>
-  <si>
-    <t>26/12/2021</t>
-  </si>
-  <si>
-    <t>27/12/2021</t>
-  </si>
-  <si>
-    <t>28/12/2021</t>
-  </si>
-  <si>
-    <t>29/12/2021</t>
-  </si>
-  <si>
-    <t>30/12/2021</t>
-  </si>
-  <si>
-    <t>31/12/2021</t>
+    <t>Program output prediction questions</t>
+  </si>
+  <si>
+    <t>Que programs from DS</t>
   </si>
 </sst>
 </file>
@@ -884,8 +866,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -907,6 +889,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -914,9 +909,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,20 +924,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -980,21 +962,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1018,8 +985,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1033,6 +1023,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -1041,23 +1038,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1072,19 +1054,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,13 +1066,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,7 +1078,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,13 +1114,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,7 +1138,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,12 +1174,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1204,37 +1186,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,13 +1204,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,15 +1245,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1317,8 +1290,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1334,6 +1307,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1355,149 +1339,147 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1840,10 +1822,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A191" sqref="A191"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A199" sqref="A199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3248,49 +3230,17 @@
         <v>276</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
-      <c r="A183" s="1" t="s">
+      <c r="C182" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
-      <c r="A184" s="1" t="s">
+    <row r="183" spans="3:3">
+      <c r="C183" s="2" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1">
-      <c r="A185" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1">
-      <c r="A186" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1">
-      <c r="A187" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1">
-      <c r="A188" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1">
-      <c r="A189" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1">
-      <c r="A190" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 24th - Status
</commit_message>
<xml_diff>
--- a/Daily_Status.xlsx
+++ b/Daily_Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8580" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="7815" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="283">
   <si>
     <t>DATE</t>
   </si>
@@ -857,6 +857,15 @@
   </si>
   <si>
     <t>Que programs from DS</t>
+  </si>
+  <si>
+    <t>24/12/2021</t>
+  </si>
+  <si>
+    <t>Gone through links and articles on OS concepts</t>
+  </si>
+  <si>
+    <t>Que programs of DS : operations</t>
   </si>
 </sst>
 </file>
@@ -864,8 +873,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -889,6 +898,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -903,29 +927,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -934,6 +943,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -993,15 +1009,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1015,31 +1047,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1054,25 +1063,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,13 +1075,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,13 +1117,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,115 +1231,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1245,6 +1254,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1296,21 +1344,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1321,165 +1354,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1822,10 +1831,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E183"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A199" sqref="A199"/>
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3241,6 +3250,17 @@
     <row r="183" spans="3:3">
       <c r="C183" s="2" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>